<commit_message>
snpGenomesFiles type update to File
</commit_message>
<xml_diff>
--- a/docs/UI/EDGE-v3-snpTree-ui.xlsx
+++ b/docs/UI/EDGE-v3-snpTree-ui.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chien-chi/Projects/LANL_git/EDGE_workflows/docs/UI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andylo/Projects/LANL/EDGEv3/docs/UI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4472C8-BCBB-E041-B054-BA8F6DBE7CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF41F8A-4005-1A46-8D6C-4CAFFFB3D9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28320" yWindow="500" windowWidth="40480" windowHeight="28300" xr2:uid="{079D525B-60B2-4B4A-BCF4-861050BE33CD}"/>
+    <workbookView xWindow="-48980" yWindow="-2340" windowWidth="30240" windowHeight="18880" xr2:uid="{079D525B-60B2-4B4A-BCF4-861050BE33CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t>yes, no</t>
   </si>
   <si>
-    <t>String? snpGenomesFiles</t>
-  </si>
-  <si>
     <t>String? snpGenomes</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>1 to 1000</t>
+  </si>
+  <si>
+    <t>File snpGenomesFiles</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,7 +750,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
@@ -760,18 +760,18 @@
         <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
@@ -835,7 +835,7 @@
         <v>100</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>

</xml_diff>